<commit_message>
first try fixing specific consumption problem. more to follow
</commit_message>
<xml_diff>
--- a/output/endemo2_gdp_prognosis.xlsx
+++ b/output/endemo2_gdp_prognosis.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42403.53</v>
+        <v>42403.5335928</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7859.68</v>
+        <v>7859.678037</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19685.49</v>
+        <v>19685.4944825</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>56563.49</v>
+        <v>56563.488473</v>
       </c>
     </row>
     <row r="6">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42973.29</v>
+        <v>42973.2899573</v>
       </c>
     </row>
     <row r="7">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>72607.63</v>
+        <v>72607.6318545</v>
       </c>
     </row>
     <row r="8">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>18647.5</v>
+        <v>18647.4957208</v>
       </c>
     </row>
     <row r="9">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27725.81</v>
+        <v>27725.8055221</v>
       </c>
     </row>
     <row r="10">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>38291.87</v>
+        <v>38291.8657809</v>
       </c>
     </row>
     <row r="11">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>13519.56</v>
+        <v>13519.5588337</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31593.48</v>
+        <v>31593.4802622</v>
       </c>
     </row>
     <row r="13">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15558.28</v>
+        <v>15558.2761098</v>
       </c>
     </row>
     <row r="14">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>107201.84</v>
+        <v>107201.8399448</v>
       </c>
     </row>
     <row r="15">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14379.44</v>
+        <v>14379.4442049</v>
       </c>
     </row>
     <row r="16">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47826.82</v>
+        <v>47826.8191173</v>
       </c>
     </row>
     <row r="17">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46188.97</v>
+        <v>46188.966512</v>
       </c>
     </row>
     <row r="18">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14332.92</v>
+        <v>14332.915891</v>
       </c>
     </row>
     <row r="19">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21057.62</v>
+        <v>21057.6174784</v>
       </c>
     </row>
     <row r="20">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10714.02</v>
+        <v>10714.0153592</v>
       </c>
     </row>
     <row r="21">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>23476.37</v>
+        <v>23476.3698862</v>
       </c>
     </row>
     <row r="22">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17730.15</v>
+        <v>17730.150113</v>
       </c>
     </row>
     <row r="23">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>45628.93</v>
+        <v>45628.9257037</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>52983.01</v>
+        <v>52983.0068617</v>
       </c>
     </row>
     <row r="25">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>47231.34</v>
+        <v>47231.3368868</v>
       </c>
     </row>
     <row r="26">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>75953.58</v>
+        <v>75953.5819515</v>
       </c>
     </row>
     <row r="27">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>87980.67</v>
+        <v>87980.67068539999</v>
       </c>
     </row>
     <row r="28">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>7381.8</v>
+        <v>7381.8041729</v>
       </c>
     </row>
     <row r="29">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5184.69</v>
+        <v>5184.6944712</v>
       </c>
     </row>
     <row r="30">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4431.54</v>
+        <v>4431.539181</v>
       </c>
     </row>
     <row r="31">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>6261.53</v>
+        <v>6261.5271391</v>
       </c>
     </row>
     <row r="32">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5387.27</v>
+        <v>5387.2696706</v>
       </c>
     </row>
     <row r="33">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>57699.46</v>
+        <v>57699.45893</v>
       </c>
     </row>
     <row r="34">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16443.59</v>
+        <v>16443.5852876</v>
       </c>
     </row>
     <row r="35">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>19677.68</v>
+        <v>19677.6768376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
specific consumption coefficients and nuts2 installed capacity output should be correct now
</commit_message>
<xml_diff>
--- a/output/endemo2_gdp_prognosis.xlsx
+++ b/output/endemo2_gdp_prognosis.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>42403.5335928</v>
+        <v>42403.53359276601</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7859.678037</v>
+        <v>7859.678037049936</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19685.4944825</v>
+        <v>19685.49448249727</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>56563.488473</v>
+        <v>56563.48847296692</v>
       </c>
     </row>
     <row r="6">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>42973.2899573</v>
+        <v>42973.28995730318</v>
       </c>
     </row>
     <row r="7">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>72607.6318545</v>
+        <v>72607.63185448138</v>
       </c>
     </row>
     <row r="8">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>18647.4957208</v>
+        <v>18647.49572075146</v>
       </c>
     </row>
     <row r="9">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27725.8055221</v>
+        <v>27725.80552207329</v>
       </c>
     </row>
     <row r="10">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>38291.8657809</v>
+        <v>38291.86578094307</v>
       </c>
     </row>
     <row r="11">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>13519.5588337</v>
+        <v>13519.55883370189</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31593.4802622</v>
+        <v>31593.48026215985</v>
       </c>
     </row>
     <row r="13">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15558.2761098</v>
+        <v>15558.27610977791</v>
       </c>
     </row>
     <row r="14">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>107201.8399448</v>
+        <v>107201.8399448164</v>
       </c>
     </row>
     <row r="15">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14379.4442049</v>
+        <v>14379.44420492945</v>
       </c>
     </row>
     <row r="16">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47826.8191173</v>
+        <v>47826.81911728431</v>
       </c>
     </row>
     <row r="17">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>46188.966512</v>
+        <v>46188.96651198716</v>
       </c>
     </row>
     <row r="18">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14332.915891</v>
+        <v>14332.91589100112</v>
       </c>
     </row>
     <row r="19">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21057.6174784</v>
+        <v>21057.61747842322</v>
       </c>
     </row>
     <row r="20">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10714.0153592</v>
+        <v>10714.0153591551</v>
       </c>
     </row>
     <row r="21">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>23476.3698862</v>
+        <v>23476.36988619294</v>
       </c>
     </row>
     <row r="22">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17730.150113</v>
+        <v>17730.15011302302</v>
       </c>
     </row>
     <row r="23">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>45628.9257037</v>
+        <v>45628.92570368129</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>52983.0068617</v>
+        <v>52983.00686174822</v>
       </c>
     </row>
     <row r="25">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>47231.3368868</v>
+        <v>47231.33688684644</v>
       </c>
     </row>
     <row r="26">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>75953.5819515</v>
+        <v>75953.58195148033</v>
       </c>
     </row>
     <row r="27">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>87980.67068539999</v>
+        <v>87980.67068543768</v>
       </c>
     </row>
     <row r="28">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>7381.8041729</v>
+        <v>7381.804172863633</v>
       </c>
     </row>
     <row r="29">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5184.6944712</v>
+        <v>5184.694471152491</v>
       </c>
     </row>
     <row r="30">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4431.539181</v>
+        <v>4431.53918098494</v>
       </c>
     </row>
     <row r="31">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>6261.5271391</v>
+        <v>6261.527139083811</v>
       </c>
     </row>
     <row r="32">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5387.2696706</v>
+        <v>5387.269670626623</v>
       </c>
     </row>
     <row r="33">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>57699.45893</v>
+        <v>57699.45892997105</v>
       </c>
     </row>
     <row r="34">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>16443.5852876</v>
+        <v>16443.58528757759</v>
       </c>
     </row>
     <row r="35">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>19677.6768376</v>
+        <v>19677.67683759608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>